<commit_message>
updated debt account formula.
</commit_message>
<xml_diff>
--- a/Personal Budget - English.xlsx
+++ b/Personal Budget - English.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcssi\Code\Personal_Finance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A79EEA-D0B5-4CF5-9F19-34399A3DE9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CBE15A-D4C2-471E-A739-438914DA6B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="792" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7948,7 +7948,7 @@
       </c>
       <c r="C7" s="81">
         <f ca="1">TODAY()</f>
-        <v>45755</v>
+        <v>45757</v>
       </c>
       <c r="E7" s="47" t="str">
         <v>Insurance</v>
@@ -8036,7 +8036,7 @@
         <v>Credit Card</v>
       </c>
       <c r="C13" s="27">
-        <f ca="1">ROUND(SUMIFS(Tabela1[Amount],Tabela1[Operation],"Expenses",Tabela1[Account],B13,Tabela1[Date],"&lt;="&amp;(IF(ISBLANK(C7),TODAY(),C7)))-SUMIFS(Tabela1[Amount],Tabela1[Category],B13,Tabela1[Date],"&lt;="&amp;(IF(ISBLANK(C7),TODAY(),C7)))+VLOOKUP(B13,'Data Validation'!$B$5:$C$10,2,FALSE),2)</f>
+        <f ca="1">ROUND(SUMIFS(Tabela1[Amount],Tabela1[Operation],"Expenses",Tabela1[Account],B13,Tabela1[Date],"&lt;="&amp;(IF(ISBLANK($C$7),TODAY(),$C$7)))-SUMIFS(Tabela1[Amount],Tabela1[Operation],"Payment",Tabela1[Category],B13,Tabela1[Date],"&lt;="&amp;(IF(ISBLANK($C$7),TODAY(),$C$7)))+VLOOKUP(B13,'Data Validation'!$B$5:$C$10,2,FALSE),2)</f>
         <v>0</v>
       </c>
       <c r="E13" s="47" t="str">

</xml_diff>